<commit_message>
Modifications done in Excel Report
</commit_message>
<xml_diff>
--- a/Playwright/Report.xlsx
+++ b/Playwright/Report.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Report" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Success</t>
   </si>
   <si>
-    <t>2023-04-05 11:34:03.528751</t>
+    <t>2023-04-05 16:42:10.901730</t>
   </si>
   <si>
     <t>v3</t>
@@ -69,29 +69,62 @@
     <t>2</t>
   </si>
   <si>
-    <t>https://jsonplaceholder.typicode.com/posts/1</t>
-  </si>
-  <si>
-    <t>2023-04-05 11:34:03.834037</t>
+    <t>https://jsonplaceholder.typicode.com/posts/getbyid</t>
+  </si>
+  <si>
+    <t>2023-04-05 16:42:11.515802</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>2023-04-05 11:34:04.817321</t>
+    <t>https://jsonplaceholder.typicode.com/posts/updatebyid</t>
+  </si>
+  <si>
+    <t>2023-04-05 16:42:12.348970</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>2023-04-05 11:34:05.756091</t>
+    <t>https://jsonplaceholder.typicode.com/posts/deletebyid</t>
+  </si>
+  <si>
+    <t>2023-04-05 16:42:13.215320</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>No.Of.Endpoints</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date Of Excecution</t>
+  </si>
+  <si>
+    <t>Api Type</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,13 +147,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,15 +198,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23474" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -543,7 +628,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -558,7 +643,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -569,10 +654,10 @@
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -587,7 +672,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -604,13 +689,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="str">
+        <f>API!I2</f>
+        <v>https://jsonplaceholder.typicode.com</v>
+      </c>
+      <c r="C2" s="6">
+        <f>COUNTA(API!A2:A5)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" s="6">
+        <f>COUNTIF(API!F2:F5, "Success")</f>
+        <v>4</v>
+      </c>
+      <c r="E2" s="6">
+        <f>COUNTIF(API!F2:F5, "Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <f>API!H2</f>
+        <v>v3</v>
+      </c>
+      <c r="G2" t="str">
+        <f>API!G2</f>
+        <v>2023-04-05 16:42:10.901730</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <f>API!I2</f>
+        <v>https://jsonplaceholder.typicode.com</v>
+      </c>
+      <c r="C7" s="10">
+        <f>COUNTIF(API!D2:D5, "User")</f>
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6">
+        <f>COUNTIFS(API!D2:D5, "User",API!F2:F5,"Success")</f>
+        <v>4</v>
+      </c>
+      <c r="F7" s="6">
+        <f>COUNTIFS(API!D2:D5, "User",API!F2:F5,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <f>SUM(E7:F7)</f>
+        <v>4</v>
+      </c>
+      <c r="H7" t="str">
+        <f>API!H2</f>
+        <v>v3</v>
+      </c>
+      <c r="I7" t="str">
+        <f>API!G2</f>
+        <v>2023-04-05 16:42:10.901730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" s="6">
+        <f>SUM(C7:C7)</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="6">
+        <f>SUM(D7:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SUM(E7:E7)</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="6">
+        <f>SUM(F7:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <f>SUM(G7:G7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="C10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 

</xml_diff>